<commit_message>
added : icon and title for page internal view
</commit_message>
<xml_diff>
--- a/data/db_source/variable.xlsx
+++ b/data/db_source/variable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64BA5EC-D37D-F94E-9465-C77DA590C4CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3B8826-2625-6247-A1EA-CCC0BACA51E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="3680" windowWidth="28800" windowHeight="14260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5236,7 +5236,7 @@
         <v>100</v>
       </c>
       <c r="E47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I47" t="s">
         <v>40</v>

</xml_diff>